<commit_message>
histograms for make histograms!
</commit_message>
<xml_diff>
--- a/TOR450 Data/5. Clean Data for Data Visualisation/TOR450_DUV_330_450_pivoted.xlsx
+++ b/TOR450 Data/5. Clean Data for Data Visualisation/TOR450_DUV_330_450_pivoted.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karina\Portfolio\TORX\TOR450 Data\5. Clean Data for Data Visualisation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FEEF75-E186-4969-B92B-9827917B78EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -4024,8 +4018,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4086,135 +4080,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4252,7 +4126,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -4286,7 +4160,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -4321,10 +4194,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4497,20 +4369,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O453"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6:O7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="15" width="17" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4557,7 +4423,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -4568,7 +4434,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -4582,7 +4448,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -4605,7 +4471,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -4616,7 +4482,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -4630,7 +4496,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -4641,7 +4507,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -4652,7 +4518,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -4660,7 +4526,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -4671,7 +4537,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -4685,7 +4551,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -4708,7 +4574,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -4737,7 +4603,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -4766,7 +4632,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -4780,7 +4646,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -4794,7 +4660,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -4805,7 +4671,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -4819,7 +4685,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -4830,7 +4696,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -4847,7 +4713,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -4858,7 +4724,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -4872,7 +4738,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -4886,7 +4752,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -4906,7 +4772,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -4920,7 +4786,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -4931,7 +4797,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -4942,7 +4808,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -4956,7 +4822,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -4967,7 +4833,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -4987,7 +4853,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -5001,7 +4867,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -5021,7 +4887,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -5041,7 +4907,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -5058,7 +4924,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -5069,7 +4935,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -5080,7 +4946,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -5091,7 +4957,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -5105,7 +4971,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -5119,7 +4985,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -5130,7 +4996,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -5141,7 +5007,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -5152,7 +5018,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -5169,7 +5035,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -5186,7 +5052,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -5200,7 +5066,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -5214,7 +5080,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -5225,7 +5091,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -5236,7 +5102,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -5250,7 +5116,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -5267,7 +5133,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -5281,7 +5147,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -5310,7 +5176,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -5321,7 +5187,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15">
       <c r="A54" t="s">
         <v>67</v>
       </c>
@@ -5332,7 +5198,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -5343,7 +5209,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -5354,7 +5220,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -5368,7 +5234,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>71</v>
       </c>
@@ -5379,7 +5245,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -5396,7 +5262,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>73</v>
       </c>
@@ -5407,7 +5273,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -5421,7 +5287,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -5438,7 +5304,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -5455,7 +5321,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -5469,7 +5335,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
         <v>78</v>
       </c>
@@ -5477,7 +5343,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -5491,7 +5357,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -5505,7 +5371,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
         <v>81</v>
       </c>
@@ -5516,7 +5382,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -5536,7 +5402,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -5547,7 +5413,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15">
       <c r="A71" t="s">
         <v>84</v>
       </c>
@@ -5558,7 +5424,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -5569,7 +5435,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -5583,7 +5449,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -5594,7 +5460,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -5608,7 +5474,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15">
       <c r="A76" t="s">
         <v>89</v>
       </c>
@@ -5616,7 +5482,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15">
       <c r="A77" t="s">
         <v>90</v>
       </c>
@@ -5627,7 +5493,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15">
       <c r="A78" t="s">
         <v>91</v>
       </c>
@@ -5638,7 +5504,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15">
       <c r="A79" t="s">
         <v>92</v>
       </c>
@@ -5652,7 +5518,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15">
       <c r="A80" t="s">
         <v>93</v>
       </c>
@@ -5663,7 +5529,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15">
       <c r="A81" t="s">
         <v>94</v>
       </c>
@@ -5671,7 +5537,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15">
       <c r="A82" t="s">
         <v>95</v>
       </c>
@@ -5685,7 +5551,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15">
       <c r="A83" t="s">
         <v>96</v>
       </c>
@@ -5696,7 +5562,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
         <v>97</v>
       </c>
@@ -5710,7 +5576,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
         <v>98</v>
       </c>
@@ -5721,7 +5587,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15">
       <c r="A86" t="s">
         <v>99</v>
       </c>
@@ -5735,7 +5601,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15">
       <c r="A87" t="s">
         <v>100</v>
       </c>
@@ -5746,7 +5612,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15">
       <c r="A88" t="s">
         <v>101</v>
       </c>
@@ -5760,7 +5626,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15">
       <c r="A89" t="s">
         <v>102</v>
       </c>
@@ -5777,7 +5643,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15">
       <c r="A90" t="s">
         <v>103</v>
       </c>
@@ -5788,7 +5654,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15">
       <c r="A91" t="s">
         <v>104</v>
       </c>
@@ -5799,7 +5665,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15">
       <c r="A92" t="s">
         <v>105</v>
       </c>
@@ -5825,7 +5691,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15">
       <c r="A93" t="s">
         <v>106</v>
       </c>
@@ -5836,7 +5702,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15">
       <c r="A94" t="s">
         <v>107</v>
       </c>
@@ -5847,7 +5713,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15">
       <c r="A95" t="s">
         <v>108</v>
       </c>
@@ -5861,7 +5727,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15">
       <c r="A96" t="s">
         <v>109</v>
       </c>
@@ -5875,7 +5741,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15">
       <c r="A97" t="s">
         <v>110</v>
       </c>
@@ -5886,7 +5752,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15">
       <c r="A98" t="s">
         <v>111</v>
       </c>
@@ -5900,7 +5766,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
         <v>112</v>
       </c>
@@ -5914,7 +5780,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15">
       <c r="A100" t="s">
         <v>113</v>
       </c>
@@ -5928,7 +5794,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15">
       <c r="A101" t="s">
         <v>114</v>
       </c>
@@ -5945,7 +5811,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15">
       <c r="A102" t="s">
         <v>115</v>
       </c>
@@ -5953,7 +5819,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15">
       <c r="A103" t="s">
         <v>116</v>
       </c>
@@ -5964,7 +5830,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15">
       <c r="A104" t="s">
         <v>117</v>
       </c>
@@ -5978,7 +5844,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15">
       <c r="A105" t="s">
         <v>118</v>
       </c>
@@ -5989,7 +5855,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15">
       <c r="A106" t="s">
         <v>119</v>
       </c>
@@ -6000,7 +5866,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15">
       <c r="A107" t="s">
         <v>120</v>
       </c>
@@ -6014,7 +5880,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15">
       <c r="A108" t="s">
         <v>121</v>
       </c>
@@ -6025,7 +5891,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15">
       <c r="A109" t="s">
         <v>122</v>
       </c>
@@ -6036,7 +5902,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15">
       <c r="A110" t="s">
         <v>123</v>
       </c>
@@ -6044,7 +5910,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15">
       <c r="A111" t="s">
         <v>124</v>
       </c>
@@ -6055,7 +5921,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15">
       <c r="A112" t="s">
         <v>125</v>
       </c>
@@ -6066,7 +5932,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15">
       <c r="A113" t="s">
         <v>126</v>
       </c>
@@ -6077,7 +5943,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15">
       <c r="A114" t="s">
         <v>127</v>
       </c>
@@ -6088,7 +5954,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15">
       <c r="A115" t="s">
         <v>128</v>
       </c>
@@ -6102,7 +5968,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15">
       <c r="A116" t="s">
         <v>129</v>
       </c>
@@ -6113,7 +5979,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15">
       <c r="A117" t="s">
         <v>130</v>
       </c>
@@ -6124,7 +5990,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15">
       <c r="A118" t="s">
         <v>131</v>
       </c>
@@ -6138,7 +6004,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15">
       <c r="A119" t="s">
         <v>132</v>
       </c>
@@ -6152,7 +6018,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15">
       <c r="A120" t="s">
         <v>133</v>
       </c>
@@ -6169,7 +6035,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15">
       <c r="A121" t="s">
         <v>134</v>
       </c>
@@ -6183,7 +6049,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15">
       <c r="A122" t="s">
         <v>135</v>
       </c>
@@ -6194,7 +6060,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15">
       <c r="A123" t="s">
         <v>136</v>
       </c>
@@ -6205,7 +6071,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15">
       <c r="A124" t="s">
         <v>137</v>
       </c>
@@ -6216,7 +6082,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15">
       <c r="A125" t="s">
         <v>138</v>
       </c>
@@ -6227,7 +6093,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15">
       <c r="A126" t="s">
         <v>139</v>
       </c>
@@ -6241,7 +6107,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15">
       <c r="A127" t="s">
         <v>140</v>
       </c>
@@ -6252,7 +6118,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15">
       <c r="A128" t="s">
         <v>141</v>
       </c>
@@ -6263,7 +6129,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15">
       <c r="A129" t="s">
         <v>142</v>
       </c>
@@ -6283,7 +6149,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15">
       <c r="A130" t="s">
         <v>143</v>
       </c>
@@ -6294,7 +6160,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15">
       <c r="A131" t="s">
         <v>144</v>
       </c>
@@ -6305,7 +6171,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15">
       <c r="A132" t="s">
         <v>145</v>
       </c>
@@ -6316,7 +6182,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15">
       <c r="A133" t="s">
         <v>146</v>
       </c>
@@ -6330,7 +6196,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15">
       <c r="A134" t="s">
         <v>147</v>
       </c>
@@ -6341,7 +6207,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15">
       <c r="A135" t="s">
         <v>148</v>
       </c>
@@ -6355,7 +6221,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15">
       <c r="A136" t="s">
         <v>149</v>
       </c>
@@ -6366,7 +6232,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15">
       <c r="A137" t="s">
         <v>150</v>
       </c>
@@ -6383,7 +6249,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15">
       <c r="A138" t="s">
         <v>151</v>
       </c>
@@ -6406,7 +6272,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15">
       <c r="A139" t="s">
         <v>152</v>
       </c>
@@ -6417,7 +6283,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15">
       <c r="A140" t="s">
         <v>153</v>
       </c>
@@ -6428,7 +6294,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15">
       <c r="A141" t="s">
         <v>154</v>
       </c>
@@ -6442,7 +6308,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15">
       <c r="A142" t="s">
         <v>155</v>
       </c>
@@ -6459,7 +6325,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15">
       <c r="A143" t="s">
         <v>156</v>
       </c>
@@ -6473,7 +6339,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15">
       <c r="A144" t="s">
         <v>157</v>
       </c>
@@ -6484,7 +6350,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15">
       <c r="A145" t="s">
         <v>158</v>
       </c>
@@ -6498,7 +6364,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15">
       <c r="A146" t="s">
         <v>159</v>
       </c>
@@ -6509,7 +6375,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15">
       <c r="A147" t="s">
         <v>160</v>
       </c>
@@ -6517,7 +6383,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15">
       <c r="A148" t="s">
         <v>161</v>
       </c>
@@ -6534,7 +6400,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15">
       <c r="A149" t="s">
         <v>162</v>
       </c>
@@ -6545,7 +6411,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15">
       <c r="A150" t="s">
         <v>163</v>
       </c>
@@ -6556,7 +6422,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15">
       <c r="A151" t="s">
         <v>164</v>
       </c>
@@ -6567,7 +6433,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15">
       <c r="A152" t="s">
         <v>165</v>
       </c>
@@ -6587,7 +6453,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15">
       <c r="A153" t="s">
         <v>166</v>
       </c>
@@ -6604,7 +6470,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15">
       <c r="A154" t="s">
         <v>167</v>
       </c>
@@ -6615,7 +6481,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15">
       <c r="A155" t="s">
         <v>168</v>
       </c>
@@ -6626,7 +6492,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15">
       <c r="A156" t="s">
         <v>169</v>
       </c>
@@ -6640,7 +6506,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15">
       <c r="A157" t="s">
         <v>170</v>
       </c>
@@ -6651,7 +6517,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15">
       <c r="A158" t="s">
         <v>171</v>
       </c>
@@ -6668,7 +6534,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15">
       <c r="A159" t="s">
         <v>172</v>
       </c>
@@ -6679,7 +6545,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15">
       <c r="A160" t="s">
         <v>173</v>
       </c>
@@ -6693,7 +6559,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15">
       <c r="A161" t="s">
         <v>174</v>
       </c>
@@ -6704,7 +6570,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15">
       <c r="A162" t="s">
         <v>175</v>
       </c>
@@ -6718,7 +6584,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15">
       <c r="A163" t="s">
         <v>176</v>
       </c>
@@ -6729,7 +6595,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15">
       <c r="A164" t="s">
         <v>177</v>
       </c>
@@ -6749,7 +6615,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15">
       <c r="A165" t="s">
         <v>178</v>
       </c>
@@ -6763,7 +6629,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15">
       <c r="A166" t="s">
         <v>179</v>
       </c>
@@ -6774,7 +6640,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15">
       <c r="A167" t="s">
         <v>180</v>
       </c>
@@ -6788,7 +6654,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15">
       <c r="A168" t="s">
         <v>181</v>
       </c>
@@ -6799,7 +6665,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15">
       <c r="A169" t="s">
         <v>182</v>
       </c>
@@ -6810,7 +6676,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15">
       <c r="A170" t="s">
         <v>183</v>
       </c>
@@ -6821,7 +6687,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15">
       <c r="A171" t="s">
         <v>184</v>
       </c>
@@ -6832,7 +6698,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15">
       <c r="A172" t="s">
         <v>185</v>
       </c>
@@ -6843,7 +6709,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15">
       <c r="A173" t="s">
         <v>186</v>
       </c>
@@ -6854,7 +6720,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15">
       <c r="A174" t="s">
         <v>187</v>
       </c>
@@ -6865,7 +6731,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15">
       <c r="A175" t="s">
         <v>188</v>
       </c>
@@ -6876,7 +6742,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15">
       <c r="A176" t="s">
         <v>189</v>
       </c>
@@ -6890,7 +6756,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15">
       <c r="A177" t="s">
         <v>190</v>
       </c>
@@ -6913,7 +6779,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15">
       <c r="A178" t="s">
         <v>191</v>
       </c>
@@ -6927,7 +6793,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15">
       <c r="A179" t="s">
         <v>192</v>
       </c>
@@ -6941,7 +6807,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15">
       <c r="A180" t="s">
         <v>193</v>
       </c>
@@ -6955,7 +6821,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15">
       <c r="A181" t="s">
         <v>194</v>
       </c>
@@ -6972,7 +6838,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15">
       <c r="A182" t="s">
         <v>195</v>
       </c>
@@ -6983,7 +6849,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15">
       <c r="A183" t="s">
         <v>196</v>
       </c>
@@ -6997,7 +6863,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15">
       <c r="A184" t="s">
         <v>197</v>
       </c>
@@ -7008,7 +6874,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15">
       <c r="A185" t="s">
         <v>198</v>
       </c>
@@ -7019,7 +6885,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15">
       <c r="A186" t="s">
         <v>199</v>
       </c>
@@ -7036,7 +6902,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15">
       <c r="A187" t="s">
         <v>200</v>
       </c>
@@ -7047,7 +6913,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15">
       <c r="A188" t="s">
         <v>201</v>
       </c>
@@ -7058,7 +6924,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15">
       <c r="A189" t="s">
         <v>202</v>
       </c>
@@ -7075,7 +6941,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15">
       <c r="A190" t="s">
         <v>203</v>
       </c>
@@ -7089,7 +6955,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15">
       <c r="A191" t="s">
         <v>204</v>
       </c>
@@ -7100,7 +6966,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15">
       <c r="A192" t="s">
         <v>205</v>
       </c>
@@ -7114,7 +6980,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15">
       <c r="A193" t="s">
         <v>206</v>
       </c>
@@ -7131,7 +6997,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15">
       <c r="A194" t="s">
         <v>207</v>
       </c>
@@ -7145,7 +7011,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15">
       <c r="A195" t="s">
         <v>208</v>
       </c>
@@ -7159,7 +7025,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15">
       <c r="A196" t="s">
         <v>209</v>
       </c>
@@ -7179,7 +7045,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15">
       <c r="A197" t="s">
         <v>210</v>
       </c>
@@ -7196,7 +7062,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15">
       <c r="A198" t="s">
         <v>211</v>
       </c>
@@ -7225,7 +7091,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15">
       <c r="A199" t="s">
         <v>212</v>
       </c>
@@ -7239,7 +7105,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15">
       <c r="A200" t="s">
         <v>213</v>
       </c>
@@ -7253,7 +7119,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15">
       <c r="A201" t="s">
         <v>214</v>
       </c>
@@ -7264,7 +7130,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15">
       <c r="A202" t="s">
         <v>215</v>
       </c>
@@ -7275,7 +7141,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15">
       <c r="A203" t="s">
         <v>216</v>
       </c>
@@ -7286,7 +7152,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15">
       <c r="A204" t="s">
         <v>217</v>
       </c>
@@ -7300,7 +7166,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15">
       <c r="A205" t="s">
         <v>218</v>
       </c>
@@ -7317,7 +7183,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15">
       <c r="A206" t="s">
         <v>219</v>
       </c>
@@ -7328,7 +7194,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15">
       <c r="A207" t="s">
         <v>220</v>
       </c>
@@ -7342,7 +7208,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15">
       <c r="A208" t="s">
         <v>221</v>
       </c>
@@ -7365,7 +7231,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15">
       <c r="A209" t="s">
         <v>222</v>
       </c>
@@ -7379,7 +7245,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15">
       <c r="A210" t="s">
         <v>223</v>
       </c>
@@ -7390,7 +7256,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15">
       <c r="A211" t="s">
         <v>224</v>
       </c>
@@ -7401,7 +7267,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15">
       <c r="A212" t="s">
         <v>225</v>
       </c>
@@ -7412,7 +7278,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15">
       <c r="A213" t="s">
         <v>226</v>
       </c>
@@ -7423,7 +7289,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15">
       <c r="A214" t="s">
         <v>227</v>
       </c>
@@ -7434,7 +7300,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15">
       <c r="A215" t="s">
         <v>228</v>
       </c>
@@ -7445,7 +7311,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15">
       <c r="A216" t="s">
         <v>229</v>
       </c>
@@ -7459,7 +7325,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15">
       <c r="A217" t="s">
         <v>230</v>
       </c>
@@ -7473,7 +7339,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15">
       <c r="A218" t="s">
         <v>231</v>
       </c>
@@ -7484,7 +7350,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15">
       <c r="A219" t="s">
         <v>232</v>
       </c>
@@ -7501,7 +7367,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15">
       <c r="A220" t="s">
         <v>233</v>
       </c>
@@ -7515,7 +7381,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15">
       <c r="A221" t="s">
         <v>234</v>
       </c>
@@ -7529,7 +7395,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15">
       <c r="A222" t="s">
         <v>235</v>
       </c>
@@ -7540,7 +7406,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15">
       <c r="A223" t="s">
         <v>236</v>
       </c>
@@ -7551,7 +7417,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15">
       <c r="A224" t="s">
         <v>237</v>
       </c>
@@ -7568,7 +7434,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15">
       <c r="A225" t="s">
         <v>238</v>
       </c>
@@ -7579,7 +7445,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15">
       <c r="A226" t="s">
         <v>239</v>
       </c>
@@ -7593,7 +7459,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15">
       <c r="A227" t="s">
         <v>240</v>
       </c>
@@ -7628,7 +7494,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15">
       <c r="A228" t="s">
         <v>241</v>
       </c>
@@ -7636,7 +7502,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15">
       <c r="A229" t="s">
         <v>242</v>
       </c>
@@ -7647,7 +7513,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15">
       <c r="A230" t="s">
         <v>243</v>
       </c>
@@ -7658,7 +7524,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15">
       <c r="A231" t="s">
         <v>244</v>
       </c>
@@ -7672,7 +7538,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15">
       <c r="A232" t="s">
         <v>245</v>
       </c>
@@ -7686,7 +7552,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15">
       <c r="A233" t="s">
         <v>246</v>
       </c>
@@ -7697,7 +7563,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15">
       <c r="A234" t="s">
         <v>247</v>
       </c>
@@ -7708,7 +7574,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15">
       <c r="A235" t="s">
         <v>248</v>
       </c>
@@ -7719,7 +7585,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15">
       <c r="A236" t="s">
         <v>249</v>
       </c>
@@ -7760,7 +7626,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15">
       <c r="A237" t="s">
         <v>250</v>
       </c>
@@ -7771,7 +7637,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15">
       <c r="A238" t="s">
         <v>251</v>
       </c>
@@ -7788,7 +7654,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15">
       <c r="A239" t="s">
         <v>252</v>
       </c>
@@ -7799,7 +7665,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15">
       <c r="A240" t="s">
         <v>253</v>
       </c>
@@ -7810,7 +7676,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15">
       <c r="A241" t="s">
         <v>254</v>
       </c>
@@ -7821,7 +7687,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15">
       <c r="A242" t="s">
         <v>255</v>
       </c>
@@ -7838,7 +7704,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15">
       <c r="A243" t="s">
         <v>256</v>
       </c>
@@ -7855,7 +7721,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15">
       <c r="A244" t="s">
         <v>257</v>
       </c>
@@ -7866,7 +7732,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15">
       <c r="A245" t="s">
         <v>258</v>
       </c>
@@ -7877,7 +7743,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15">
       <c r="A246" t="s">
         <v>259</v>
       </c>
@@ -7891,7 +7757,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15">
       <c r="A247" t="s">
         <v>260</v>
       </c>
@@ -7908,7 +7774,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15">
       <c r="A248" t="s">
         <v>261</v>
       </c>
@@ -7919,7 +7785,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15">
       <c r="A249" t="s">
         <v>262</v>
       </c>
@@ -7933,7 +7799,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15">
       <c r="A250" t="s">
         <v>263</v>
       </c>
@@ -7950,7 +7816,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15">
       <c r="A251" t="s">
         <v>264</v>
       </c>
@@ -7961,7 +7827,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15">
       <c r="A252" t="s">
         <v>265</v>
       </c>
@@ -7972,7 +7838,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15">
       <c r="A253" t="s">
         <v>266</v>
       </c>
@@ -7986,7 +7852,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15">
       <c r="A254" t="s">
         <v>267</v>
       </c>
@@ -8021,7 +7887,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15">
       <c r="A255" t="s">
         <v>268</v>
       </c>
@@ -8041,7 +7907,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15">
       <c r="A256" t="s">
         <v>269</v>
       </c>
@@ -8058,7 +7924,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15">
       <c r="A257" t="s">
         <v>270</v>
       </c>
@@ -8072,7 +7938,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15">
       <c r="A258" t="s">
         <v>271</v>
       </c>
@@ -8083,7 +7949,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15">
       <c r="A259" t="s">
         <v>272</v>
       </c>
@@ -8094,7 +7960,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15">
       <c r="A260" t="s">
         <v>273</v>
       </c>
@@ -8105,7 +7971,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15">
       <c r="A261" t="s">
         <v>274</v>
       </c>
@@ -8119,7 +7985,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15">
       <c r="A262" t="s">
         <v>275</v>
       </c>
@@ -8130,7 +7996,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15">
       <c r="A263" t="s">
         <v>276</v>
       </c>
@@ -8144,7 +8010,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15">
       <c r="A264" t="s">
         <v>277</v>
       </c>
@@ -8161,7 +8027,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15">
       <c r="A265" t="s">
         <v>278</v>
       </c>
@@ -8172,7 +8038,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15">
       <c r="A266" t="s">
         <v>279</v>
       </c>
@@ -8183,7 +8049,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15">
       <c r="A267" t="s">
         <v>280</v>
       </c>
@@ -8194,7 +8060,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15">
       <c r="A268" t="s">
         <v>281</v>
       </c>
@@ -8205,7 +8071,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15">
       <c r="A269" t="s">
         <v>282</v>
       </c>
@@ -8216,7 +8082,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15">
       <c r="A270" t="s">
         <v>283</v>
       </c>
@@ -8227,7 +8093,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15">
       <c r="A271" t="s">
         <v>284</v>
       </c>
@@ -8253,7 +8119,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15">
       <c r="A272" t="s">
         <v>285</v>
       </c>
@@ -8270,7 +8136,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15">
       <c r="A273" t="s">
         <v>286</v>
       </c>
@@ -8281,7 +8147,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15">
       <c r="A274" t="s">
         <v>287</v>
       </c>
@@ -8292,7 +8158,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15">
       <c r="A275" t="s">
         <v>288</v>
       </c>
@@ -8309,7 +8175,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15">
       <c r="A276" t="s">
         <v>289</v>
       </c>
@@ -8323,7 +8189,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15">
       <c r="A277" t="s">
         <v>290</v>
       </c>
@@ -8334,7 +8200,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15">
       <c r="A278" t="s">
         <v>291</v>
       </c>
@@ -8351,7 +8217,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15">
       <c r="A279" t="s">
         <v>292</v>
       </c>
@@ -8362,7 +8228,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15">
       <c r="A280" t="s">
         <v>293</v>
       </c>
@@ -8373,7 +8239,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15">
       <c r="A281" t="s">
         <v>294</v>
       </c>
@@ -8387,7 +8253,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15">
       <c r="A282" t="s">
         <v>295</v>
       </c>
@@ -8404,7 +8270,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15">
       <c r="A283" t="s">
         <v>296</v>
       </c>
@@ -8424,7 +8290,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15">
       <c r="A284" t="s">
         <v>297</v>
       </c>
@@ -8435,7 +8301,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15">
       <c r="A285" t="s">
         <v>298</v>
       </c>
@@ -8446,7 +8312,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15">
       <c r="A286" t="s">
         <v>299</v>
       </c>
@@ -8460,7 +8326,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15">
       <c r="A287" t="s">
         <v>300</v>
       </c>
@@ -8471,7 +8337,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15">
       <c r="A288" t="s">
         <v>301</v>
       </c>
@@ -8485,7 +8351,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15">
       <c r="A289" t="s">
         <v>302</v>
       </c>
@@ -8499,7 +8365,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15">
       <c r="A290" t="s">
         <v>303</v>
       </c>
@@ -8513,7 +8379,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:15">
       <c r="A291" t="s">
         <v>304</v>
       </c>
@@ -8524,7 +8390,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15">
       <c r="A292" t="s">
         <v>305</v>
       </c>
@@ -8541,7 +8407,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15">
       <c r="A293" t="s">
         <v>306</v>
       </c>
@@ -8552,7 +8418,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15">
       <c r="A294" t="s">
         <v>307</v>
       </c>
@@ -8563,7 +8429,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="295" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15">
       <c r="A295" t="s">
         <v>308</v>
       </c>
@@ -8583,7 +8449,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="296" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15">
       <c r="A296" t="s">
         <v>309</v>
       </c>
@@ -8600,7 +8466,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="297" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:15">
       <c r="A297" t="s">
         <v>310</v>
       </c>
@@ -8620,7 +8486,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:15">
       <c r="A298" t="s">
         <v>311</v>
       </c>
@@ -8631,7 +8497,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15">
       <c r="A299" t="s">
         <v>312</v>
       </c>
@@ -8642,7 +8508,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="300" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:15">
       <c r="A300" t="s">
         <v>313</v>
       </c>
@@ -8665,7 +8531,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:15">
       <c r="A301" t="s">
         <v>314</v>
       </c>
@@ -8679,7 +8545,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="302" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:15">
       <c r="A302" t="s">
         <v>315</v>
       </c>
@@ -8702,7 +8568,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="303" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:15">
       <c r="A303" t="s">
         <v>316</v>
       </c>
@@ -8713,7 +8579,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="304" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15">
       <c r="A304" t="s">
         <v>317</v>
       </c>
@@ -8733,7 +8599,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="305" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:15">
       <c r="A305" t="s">
         <v>318</v>
       </c>
@@ -8747,7 +8613,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="306" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:15">
       <c r="A306" t="s">
         <v>319</v>
       </c>
@@ -8758,7 +8624,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="307" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:15">
       <c r="A307" t="s">
         <v>320</v>
       </c>
@@ -8772,7 +8638,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="308" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:15">
       <c r="A308" t="s">
         <v>321</v>
       </c>
@@ -8789,7 +8655,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="309" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:15">
       <c r="A309" t="s">
         <v>322</v>
       </c>
@@ -8800,7 +8666,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="310" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:15">
       <c r="A310" t="s">
         <v>323</v>
       </c>
@@ -8817,7 +8683,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="311" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:15">
       <c r="A311" t="s">
         <v>324</v>
       </c>
@@ -8828,7 +8694,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="312" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:15">
       <c r="A312" t="s">
         <v>325</v>
       </c>
@@ -8839,7 +8705,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="313" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:15">
       <c r="A313" t="s">
         <v>326</v>
       </c>
@@ -8856,7 +8722,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="314" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:15">
       <c r="A314" t="s">
         <v>327</v>
       </c>
@@ -8864,7 +8730,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="315" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:15">
       <c r="A315" t="s">
         <v>328</v>
       </c>
@@ -8890,7 +8756,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="316" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:15">
       <c r="A316" t="s">
         <v>329</v>
       </c>
@@ -8901,7 +8767,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="317" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:15">
       <c r="A317" t="s">
         <v>330</v>
       </c>
@@ -8921,7 +8787,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="318" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:15">
       <c r="A318" t="s">
         <v>331</v>
       </c>
@@ -8932,7 +8798,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="319" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:15">
       <c r="A319" t="s">
         <v>332</v>
       </c>
@@ -8955,7 +8821,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="320" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:15">
       <c r="A320" t="s">
         <v>333</v>
       </c>
@@ -8966,7 +8832,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="321" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:15">
       <c r="A321" t="s">
         <v>334</v>
       </c>
@@ -8977,7 +8843,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="322" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:15">
       <c r="A322" t="s">
         <v>335</v>
       </c>
@@ -8994,7 +8860,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="323" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:15">
       <c r="A323" t="s">
         <v>336</v>
       </c>
@@ -9014,7 +8880,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="324" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:15">
       <c r="A324" t="s">
         <v>337</v>
       </c>
@@ -9028,7 +8894,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="325" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:15">
       <c r="A325" t="s">
         <v>338</v>
       </c>
@@ -9039,7 +8905,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:15">
       <c r="A326" t="s">
         <v>339</v>
       </c>
@@ -9062,7 +8928,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="327" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:15">
       <c r="A327" t="s">
         <v>340</v>
       </c>
@@ -9082,7 +8948,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="328" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:15">
       <c r="A328" t="s">
         <v>341</v>
       </c>
@@ -9099,7 +8965,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="329" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:15">
       <c r="A329" t="s">
         <v>342</v>
       </c>
@@ -9122,7 +8988,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="330" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:15">
       <c r="A330" t="s">
         <v>343</v>
       </c>
@@ -9136,7 +9002,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="331" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:15">
       <c r="A331" t="s">
         <v>344</v>
       </c>
@@ -9150,7 +9016,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="332" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:15">
       <c r="A332" t="s">
         <v>345</v>
       </c>
@@ -9161,7 +9027,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="333" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:15">
       <c r="A333" t="s">
         <v>346</v>
       </c>
@@ -9175,7 +9041,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="334" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:15">
       <c r="A334" t="s">
         <v>347</v>
       </c>
@@ -9186,7 +9052,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="335" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:15">
       <c r="A335" t="s">
         <v>348</v>
       </c>
@@ -9203,7 +9069,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="336" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:15">
       <c r="A336" t="s">
         <v>349</v>
       </c>
@@ -9214,7 +9080,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="337" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:15">
       <c r="A337" t="s">
         <v>350</v>
       </c>
@@ -9228,7 +9094,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="338" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:15">
       <c r="A338" t="s">
         <v>351</v>
       </c>
@@ -9242,7 +9108,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="339" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:15">
       <c r="A339" t="s">
         <v>352</v>
       </c>
@@ -9262,7 +9128,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="340" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:15">
       <c r="A340" t="s">
         <v>353</v>
       </c>
@@ -9273,7 +9139,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="341" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:15">
       <c r="A341" t="s">
         <v>354</v>
       </c>
@@ -9284,7 +9150,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="342" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:15">
       <c r="A342" t="s">
         <v>355</v>
       </c>
@@ -9295,7 +9161,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="343" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:15">
       <c r="A343" t="s">
         <v>356</v>
       </c>
@@ -9327,7 +9193,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="344" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:15">
       <c r="A344" t="s">
         <v>357</v>
       </c>
@@ -9341,7 +9207,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="345" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:15">
       <c r="A345" t="s">
         <v>358</v>
       </c>
@@ -9352,7 +9218,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="346" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:15">
       <c r="A346" t="s">
         <v>359</v>
       </c>
@@ -9378,7 +9244,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="347" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:15">
       <c r="A347" t="s">
         <v>360</v>
       </c>
@@ -9389,7 +9255,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="348" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:15">
       <c r="A348" t="s">
         <v>361</v>
       </c>
@@ -9400,7 +9266,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="349" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:15">
       <c r="A349" t="s">
         <v>362</v>
       </c>
@@ -9411,7 +9277,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="350" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:15">
       <c r="A350" t="s">
         <v>363</v>
       </c>
@@ -9428,7 +9294,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="351" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:15">
       <c r="A351" t="s">
         <v>364</v>
       </c>
@@ -9439,7 +9305,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="352" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:15">
       <c r="A352" t="s">
         <v>365</v>
       </c>
@@ -9450,7 +9316,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="353" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:15">
       <c r="A353" t="s">
         <v>366</v>
       </c>
@@ -9467,7 +9333,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="354" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:15">
       <c r="A354" t="s">
         <v>367</v>
       </c>
@@ -9490,7 +9356,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="355" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:15">
       <c r="A355" t="s">
         <v>368</v>
       </c>
@@ -9507,7 +9373,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="356" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:15">
       <c r="A356" t="s">
         <v>369</v>
       </c>
@@ -9521,7 +9387,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="357" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:15">
       <c r="A357" t="s">
         <v>370</v>
       </c>
@@ -9535,7 +9401,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="358" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:15">
       <c r="A358" t="s">
         <v>371</v>
       </c>
@@ -9546,7 +9412,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="359" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:15">
       <c r="A359" t="s">
         <v>372</v>
       </c>
@@ -9557,7 +9423,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="360" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:15">
       <c r="A360" t="s">
         <v>373</v>
       </c>
@@ -9571,7 +9437,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="361" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:15">
       <c r="A361" t="s">
         <v>374</v>
       </c>
@@ -9582,7 +9448,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="362" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:15">
       <c r="A362" t="s">
         <v>375</v>
       </c>
@@ -9611,7 +9477,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="363" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:15">
       <c r="A363" t="s">
         <v>376</v>
       </c>
@@ -9628,7 +9494,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="364" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:15">
       <c r="A364" t="s">
         <v>377</v>
       </c>
@@ -9645,7 +9511,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="365" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:15">
       <c r="A365" t="s">
         <v>378</v>
       </c>
@@ -9656,7 +9522,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="366" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:15">
       <c r="A366" t="s">
         <v>379</v>
       </c>
@@ -9673,7 +9539,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="367" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:15">
       <c r="A367" t="s">
         <v>380</v>
       </c>
@@ -9684,7 +9550,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="368" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:15">
       <c r="A368" t="s">
         <v>381</v>
       </c>
@@ -9698,7 +9564,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="369" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:15">
       <c r="A369" t="s">
         <v>382</v>
       </c>
@@ -9712,7 +9578,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="370" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:15">
       <c r="A370" t="s">
         <v>383</v>
       </c>
@@ -9720,7 +9586,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="371" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:15">
       <c r="A371" t="s">
         <v>384</v>
       </c>
@@ -9731,7 +9597,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="372" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:15">
       <c r="A372" t="s">
         <v>385</v>
       </c>
@@ -9745,7 +9611,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="373" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:15">
       <c r="A373" t="s">
         <v>386</v>
       </c>
@@ -9774,7 +9640,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="374" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:15">
       <c r="A374" t="s">
         <v>387</v>
       </c>
@@ -9788,7 +9654,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="375" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:15">
       <c r="A375" t="s">
         <v>388</v>
       </c>
@@ -9799,7 +9665,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="376" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:15">
       <c r="A376" t="s">
         <v>389</v>
       </c>
@@ -9813,7 +9679,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="377" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:15">
       <c r="A377" t="s">
         <v>390</v>
       </c>
@@ -9824,7 +9690,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="378" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:15">
       <c r="A378" t="s">
         <v>391</v>
       </c>
@@ -9838,7 +9704,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="379" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:15">
       <c r="A379" t="s">
         <v>392</v>
       </c>
@@ -9849,7 +9715,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="380" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:15">
       <c r="A380" t="s">
         <v>393</v>
       </c>
@@ -9860,7 +9726,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="381" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:15">
       <c r="A381" t="s">
         <v>394</v>
       </c>
@@ -9874,7 +9740,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="382" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:15">
       <c r="A382" t="s">
         <v>395</v>
       </c>
@@ -9891,7 +9757,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="383" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:15">
       <c r="A383" t="s">
         <v>396</v>
       </c>
@@ -9902,7 +9768,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="384" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:15">
       <c r="A384" t="s">
         <v>397</v>
       </c>
@@ -9916,7 +9782,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="385" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:15">
       <c r="A385" t="s">
         <v>398</v>
       </c>
@@ -9927,7 +9793,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="386" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:15">
       <c r="A386" t="s">
         <v>399</v>
       </c>
@@ -9938,7 +9804,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="387" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:15">
       <c r="A387" t="s">
         <v>400</v>
       </c>
@@ -9949,7 +9815,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="388" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:15">
       <c r="A388" t="s">
         <v>401</v>
       </c>
@@ -9960,7 +9826,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="389" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:15">
       <c r="A389" t="s">
         <v>402</v>
       </c>
@@ -9977,7 +9843,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="390" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:15">
       <c r="A390" t="s">
         <v>403</v>
       </c>
@@ -9994,7 +9860,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="391" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:15">
       <c r="A391" t="s">
         <v>404</v>
       </c>
@@ -10011,7 +9877,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="392" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:15">
       <c r="A392" t="s">
         <v>405</v>
       </c>
@@ -10025,7 +9891,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="393" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:15">
       <c r="A393" t="s">
         <v>406</v>
       </c>
@@ -10039,7 +9905,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="394" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:15">
       <c r="A394" t="s">
         <v>407</v>
       </c>
@@ -10050,7 +9916,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="395" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:15">
       <c r="A395" t="s">
         <v>408</v>
       </c>
@@ -10070,7 +9936,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="396" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:15">
       <c r="A396" t="s">
         <v>409</v>
       </c>
@@ -10084,7 +9950,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="397" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:15">
       <c r="A397" t="s">
         <v>410</v>
       </c>
@@ -10095,7 +9961,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="398" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:15">
       <c r="A398" t="s">
         <v>411</v>
       </c>
@@ -10106,7 +9972,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="399" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:15">
       <c r="A399" t="s">
         <v>412</v>
       </c>
@@ -10120,7 +9986,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="400" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:15">
       <c r="A400" t="s">
         <v>413</v>
       </c>
@@ -10134,7 +10000,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="401" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:15">
       <c r="A401" t="s">
         <v>414</v>
       </c>
@@ -10175,7 +10041,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="402" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:15">
       <c r="A402" t="s">
         <v>415</v>
       </c>
@@ -10186,7 +10052,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="403" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:15">
       <c r="A403" t="s">
         <v>416</v>
       </c>
@@ -10194,7 +10060,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="404" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:15">
       <c r="A404" t="s">
         <v>417</v>
       </c>
@@ -10205,7 +10071,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="405" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:15">
       <c r="A405" t="s">
         <v>418</v>
       </c>
@@ -10225,7 +10091,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="406" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:15">
       <c r="A406" t="s">
         <v>419</v>
       </c>
@@ -10239,7 +10105,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="407" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:15">
       <c r="A407" t="s">
         <v>420</v>
       </c>
@@ -10250,7 +10116,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="408" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:15">
       <c r="A408" t="s">
         <v>421</v>
       </c>
@@ -10264,7 +10130,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="409" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:15">
       <c r="A409" t="s">
         <v>422</v>
       </c>
@@ -10278,7 +10144,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="410" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:15">
       <c r="A410" t="s">
         <v>423</v>
       </c>
@@ -10292,7 +10158,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="411" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:15">
       <c r="A411" t="s">
         <v>424</v>
       </c>
@@ -10306,7 +10172,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="412" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:15">
       <c r="A412" t="s">
         <v>425</v>
       </c>
@@ -10317,7 +10183,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="413" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:15">
       <c r="A413" t="s">
         <v>426</v>
       </c>
@@ -10331,7 +10197,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="414" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:15">
       <c r="A414" t="s">
         <v>427</v>
       </c>
@@ -10351,7 +10217,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="415" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:15">
       <c r="A415" t="s">
         <v>428</v>
       </c>
@@ -10368,7 +10234,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="416" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:15">
       <c r="A416" t="s">
         <v>429</v>
       </c>
@@ -10391,7 +10257,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="417" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:15">
       <c r="A417" t="s">
         <v>430</v>
       </c>
@@ -10405,7 +10271,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="418" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:15">
       <c r="A418" t="s">
         <v>431</v>
       </c>
@@ -10422,7 +10288,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="419" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:15">
       <c r="A419" t="s">
         <v>432</v>
       </c>
@@ -10436,7 +10302,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="420" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:15">
       <c r="A420" t="s">
         <v>433</v>
       </c>
@@ -10453,7 +10319,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="421" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:15">
       <c r="A421" t="s">
         <v>434</v>
       </c>
@@ -10476,7 +10342,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="422" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:15">
       <c r="A422" t="s">
         <v>435</v>
       </c>
@@ -10493,7 +10359,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="423" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:15">
       <c r="A423" t="s">
         <v>436</v>
       </c>
@@ -10513,7 +10379,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="424" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:15">
       <c r="A424" t="s">
         <v>437</v>
       </c>
@@ -10533,7 +10399,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="425" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:15">
       <c r="A425" t="s">
         <v>438</v>
       </c>
@@ -10553,7 +10419,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="426" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:15">
       <c r="A426" t="s">
         <v>439</v>
       </c>
@@ -10564,7 +10430,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="427" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:15">
       <c r="A427" t="s">
         <v>440</v>
       </c>
@@ -10575,7 +10441,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="428" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:15">
       <c r="A428" t="s">
         <v>441</v>
       </c>
@@ -10586,7 +10452,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="429" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:15">
       <c r="A429" t="s">
         <v>442</v>
       </c>
@@ -10600,7 +10466,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="430" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:15">
       <c r="A430" t="s">
         <v>443</v>
       </c>
@@ -10611,7 +10477,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="431" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:15">
       <c r="A431" t="s">
         <v>444</v>
       </c>
@@ -10634,7 +10500,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="432" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:15">
       <c r="A432" t="s">
         <v>445</v>
       </c>
@@ -10642,7 +10508,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="433" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:15">
       <c r="A433" t="s">
         <v>446</v>
       </c>
@@ -10653,7 +10519,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="434" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:15">
       <c r="A434" t="s">
         <v>447</v>
       </c>
@@ -10664,7 +10530,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="435" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:15">
       <c r="A435" t="s">
         <v>448</v>
       </c>
@@ -10675,7 +10541,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="436" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:15">
       <c r="A436" t="s">
         <v>449</v>
       </c>
@@ -10686,7 +10552,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="437" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:15">
       <c r="A437" t="s">
         <v>450</v>
       </c>
@@ -10697,7 +10563,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="438" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:15">
       <c r="A438" t="s">
         <v>451</v>
       </c>
@@ -10708,7 +10574,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="439" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:15">
       <c r="A439" t="s">
         <v>452</v>
       </c>
@@ -10719,7 +10585,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="440" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:15">
       <c r="A440" t="s">
         <v>453</v>
       </c>
@@ -10730,7 +10596,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="441" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:15">
       <c r="A441" t="s">
         <v>454</v>
       </c>
@@ -10741,7 +10607,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="442" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:15">
       <c r="A442" t="s">
         <v>455</v>
       </c>
@@ -10752,7 +10618,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="443" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:15">
       <c r="A443" t="s">
         <v>456</v>
       </c>
@@ -10772,7 +10638,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="444" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:15">
       <c r="A444" t="s">
         <v>457</v>
       </c>
@@ -10783,7 +10649,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="445" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:15">
       <c r="A445" t="s">
         <v>458</v>
       </c>
@@ -10794,7 +10660,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="446" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:15">
       <c r="A446" t="s">
         <v>459</v>
       </c>
@@ -10808,7 +10674,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="447" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:15">
       <c r="A447" t="s">
         <v>460</v>
       </c>
@@ -10822,7 +10688,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="448" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:15">
       <c r="A448" t="s">
         <v>461</v>
       </c>
@@ -10833,7 +10699,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="449" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:15">
       <c r="A449" t="s">
         <v>462</v>
       </c>
@@ -10844,7 +10710,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="450" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:15">
       <c r="A450" t="s">
         <v>463</v>
       </c>
@@ -10855,7 +10721,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="451" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:15">
       <c r="A451" t="s">
         <v>464</v>
       </c>
@@ -10866,7 +10732,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="452" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:15">
       <c r="A452" t="s">
         <v>465</v>
       </c>
@@ -10877,7 +10743,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="453" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:15">
       <c r="A453" t="s">
         <v>466</v>
       </c>
@@ -10892,25 +10758,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:O453">
-    <cfRule type="containsText" dxfId="5" priority="6" stopIfTrue="1" operator="containsText" text="TOR450 DNF">
-      <formula>NOT(ISERROR(SEARCH("TOR450 DNF",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="1" stopIfTrue="1" operator="containsText" text="TOR450 DNF">
-      <formula>NOT(ISERROR(SEARCH("TOR450 DNF",A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="tor450">
-      <formula>NOT(ISERROR(SEARCH("tor450",A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29:F30">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="tor450 DNF">
-      <formula>NOT(ISERROR(SEARCH("tor450 DNF",E29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>